<commit_message>
new model (second ten data points)
</commit_message>
<xml_diff>
--- a/src/main/shoot_model/DataPts.xlsx
+++ b/src/main/shoot_model/DataPts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krishiyengar/AKRS_Apps/Robo/Crescendo2024/src/main/shoot_model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B09DE3-AF48-C24E-9D36-1863DD9BE10E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{403106F0-8BCE-3240-86B7-ACC7AEB747A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="19120" windowHeight="17440" xr2:uid="{84FFF492-AC58-9E46-ACA0-4E4AF797DEDA}"/>
   </bookViews>
@@ -54,16 +54,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -98,10 +90,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,314 +407,313 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0382AEAB-B36F-9541-8466-A87ECB72D1D9}">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>-4.1399999999999997</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="C2" s="1">
+        <v>70</v>
+      </c>
+      <c r="D2" s="1">
+        <v>-0.02</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>-3.2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>70</v>
+      </c>
+      <c r="D3" s="1">
+        <v>-0.02</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>6.53</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.31</v>
+      </c>
+      <c r="C4" s="1">
+        <v>70</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>1.28</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="C5" s="1">
+        <v>70</v>
+      </c>
+      <c r="D5" s="1">
+        <v>-1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>-8.51</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="C6" s="1">
+        <v>80</v>
+      </c>
+      <c r="D6" s="1">
+        <v>-3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>-11.61</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.108</v>
+      </c>
+      <c r="C7" s="1">
+        <v>90</v>
+      </c>
+      <c r="D7" s="1">
+        <v>-4.1500000000000002E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>-12.34</v>
+      </c>
+      <c r="B8" s="1">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="C8" s="1">
+        <v>90</v>
+      </c>
+      <c r="D8" s="1">
+        <v>-4.2999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>-12.41</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C9" s="1">
+        <v>90</v>
+      </c>
+      <c r="D9" s="1">
+        <v>-0.04</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>-3.3</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="C10" s="1">
+        <v>80</v>
+      </c>
+      <c r="D10" s="1">
+        <v>-2.2499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>-0.11</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.248</v>
+      </c>
+      <c r="C11" s="1">
+        <v>70</v>
+      </c>
+      <c r="D11" s="1">
+        <v>-5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
         <v>-5.5</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B13" s="1">
         <v>0.19</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C13" s="1">
         <v>80</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D13" s="1">
         <v>-1.5100000000000001E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
         <v>5.5</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B14" s="1">
         <v>0.24</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C14" s="1">
         <v>50</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D14" s="1">
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
         <v>-13.8</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B15" s="1">
         <v>0.05</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C15" s="1">
         <v>95</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D15" s="1">
         <v>-3.6999999999999998E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
         <v>-6.2</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B16" s="1">
         <v>0.14000000000000001</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C16" s="1">
         <v>70</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D16" s="1">
         <v>-0.02</v>
       </c>
-      <c r="K5" s="1"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
         <v>4.5999999999999996</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B17" s="1">
         <v>0.21</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C17" s="1">
         <v>60</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D17" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
         <v>8.6</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B18" s="1">
         <v>0.31</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C18" s="1">
         <v>60</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D18" s="1">
         <v>0.02</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
         <v>16.600000000000001</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B19" s="1">
         <v>0.33</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C19" s="1">
         <v>60</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D19" s="1">
         <v>0.03</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
         <v>-7.3</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B20" s="1">
         <v>0.12</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C20" s="1">
         <v>75</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D20" s="1">
         <v>-2.75E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
         <v>-1.8</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B21" s="1">
         <v>0.19</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C21" s="1">
         <v>75</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D21" s="1">
         <v>-1.7500000000000002E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
         <v>-6.4</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B22" s="1">
         <v>0.13</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C22" s="1">
         <v>90</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D22" s="1">
         <v>-2.2499999999999999E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
-        <v>-4.1399999999999997</v>
-      </c>
-      <c r="B12" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="C12" s="2">
-        <v>70</v>
-      </c>
-      <c r="D12" s="2">
-        <v>-0.02</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
-        <v>-3.2</v>
-      </c>
-      <c r="B13" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="C13" s="2">
-        <v>70</v>
-      </c>
-      <c r="D13" s="2">
-        <v>-0.02</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
-        <v>6.53</v>
-      </c>
-      <c r="B14" s="2">
-        <v>0.31</v>
-      </c>
-      <c r="C14" s="2">
-        <v>70</v>
-      </c>
-      <c r="D14" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
-        <v>1.28</v>
-      </c>
-      <c r="B15" s="2">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="C15" s="2">
-        <v>70</v>
-      </c>
-      <c r="D15" s="2">
-        <v>-1.4999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
-        <v>-8.51</v>
-      </c>
-      <c r="B16" s="2">
-        <v>0.13100000000000001</v>
-      </c>
-      <c r="C16" s="2">
-        <v>80</v>
-      </c>
-      <c r="D16" s="2">
-        <v>-3.5000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
-        <v>-11.61</v>
-      </c>
-      <c r="B17" s="2">
-        <v>0.108</v>
-      </c>
-      <c r="C17" s="2">
-        <v>90</v>
-      </c>
-      <c r="D17" s="2">
-        <v>-4.1500000000000002E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
-        <v>-12.34</v>
-      </c>
-      <c r="B18" s="2">
-        <v>9.6000000000000002E-2</v>
-      </c>
-      <c r="C18" s="2">
-        <v>90</v>
-      </c>
-      <c r="D18" s="2">
-        <v>-4.2999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
-        <v>-12.41</v>
-      </c>
-      <c r="B19" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="C19" s="2">
-        <v>90</v>
-      </c>
-      <c r="D19" s="2">
-        <v>-0.04</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
-        <v>-3.3</v>
-      </c>
-      <c r="B20" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="C20" s="2">
-        <v>80</v>
-      </c>
-      <c r="D20" s="2">
-        <v>-2.2499999999999999E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
-        <v>-0.11</v>
-      </c>
-      <c r="B21" s="2">
-        <v>0.248</v>
-      </c>
-      <c r="C21" s="2">
-        <v>70</v>
-      </c>
-      <c r="D21" s="2">
-        <v>-5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>